<commit_message>
Checked assumptions of linear model for algal overgrowth over coral size. Ran ANCOVA on overgrowth by coral area with algae and sponge as groups.
</commit_message>
<xml_diff>
--- a/Data/coral_allometry.xlsx
+++ b/Data/coral_allometry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NinaBean/Documents/Documents - MacBook Air/Projects/Benthic_interactions/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4080AFF5-CE6D-1948-948E-02D61B503B05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2F4F4F-B5AF-1449-95BA-B94E4CCC7F54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="28780" windowHeight="16940" activeTab="1" xr2:uid="{DE78F73A-D534-9546-B3D9-3A553E9BB58D}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28780" windowHeight="16940" xr2:uid="{DE78F73A-D534-9546-B3D9-3A553E9BB58D}"/>
   </bookViews>
   <sheets>
     <sheet name="Field" sheetId="1" r:id="rId1"/>
@@ -830,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -845,6 +845,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1161,10 +1162,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{361E3A6B-3B86-0443-BFA2-262CCB179B06}">
   <dimension ref="A1:Y488"/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A425" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A415" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D457" sqref="D457"/>
+      <selection pane="bottomLeft" activeCell="I433" sqref="I433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21856,9 +21857,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB1D9C6-A734-B745-A998-D4DE37DC140B}">
   <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P41" sqref="P41"/>
+    <sheetView zoomScale="107" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22739,8 +22740,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="8">
+    <row r="26" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
         <v>5476</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -22749,54 +22750,54 @@
       <c r="C26" s="6">
         <v>19</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="6">
         <v>350</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="6">
         <v>15</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H26" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I26" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="J26" s="8">
+      <c r="I26" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="J26" s="6">
         <v>113</v>
       </c>
-      <c r="K26" s="8">
+      <c r="K26" s="6">
         <v>92</v>
       </c>
-      <c r="L26" s="8">
+      <c r="L26" s="6">
         <v>49</v>
       </c>
-      <c r="M26" s="8">
+      <c r="M26" s="6">
         <v>14</v>
       </c>
-      <c r="N26" s="8">
+      <c r="N26" s="6">
         <v>4</v>
       </c>
-      <c r="O26" s="8" t="s">
+      <c r="O26" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="P26" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q26" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="R26" s="8" t="s">
+      <c r="P26" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q26" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="R26" s="6" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="8">
+    <row r="27" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
         <v>5476</v>
       </c>
       <c r="B27" s="6" t="s">
@@ -22805,42 +22806,42 @@
       <c r="C27" s="6">
         <v>19</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="6">
         <v>56</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G27" s="8">
-        <v>55</v>
-      </c>
-      <c r="H27" s="8" t="s">
+      <c r="G27" s="6">
+        <v>55</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="I27" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="M27" s="8">
+      <c r="I27" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="M27" s="6">
         <v>39</v>
       </c>
-      <c r="N27" s="8">
+      <c r="N27" s="6">
         <v>24</v>
       </c>
-      <c r="O27" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="P27" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q27" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="8">
+      <c r="O27" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q27" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
         <v>5476</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -22849,36 +22850,36 @@
       <c r="C28" s="6">
         <v>19</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="6">
         <v>21</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="H28" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I28" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="M28" s="8">
+      <c r="I28" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="M28" s="6">
         <v>18</v>
       </c>
-      <c r="N28" s="8">
-        <v>7</v>
-      </c>
-      <c r="O28" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="P28" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q28" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="8">
+      <c r="N28" s="6">
+        <v>7</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="P28" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q28" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
         <v>5476</v>
       </c>
       <c r="B29" s="6" t="s">
@@ -22887,24 +22888,24 @@
       <c r="C29" s="6">
         <v>19</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="6">
         <v>35</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H29" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="I29" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q29" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="8">
+      <c r="I29" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q29" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
         <v>5476</v>
       </c>
       <c r="B30" s="6" t="s">
@@ -22913,247 +22914,247 @@
       <c r="C30" s="6">
         <v>19</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="6">
         <v>19</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I30" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q30" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I30" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q30" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>5476</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="8">
         <v>19</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="14">
         <f>340+32</f>
         <v>372</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="14">
         <v>14</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="I31" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J31" s="2">
+      <c r="I31" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J31" s="14">
         <v>113</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="14">
         <v>95</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L31" s="14">
         <v>73</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M31" s="14">
         <v>38</v>
       </c>
-      <c r="N31" s="2">
+      <c r="N31" s="14">
         <v>19</v>
       </c>
-      <c r="O31" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P31" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q31" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="R31" s="5" t="s">
+      <c r="O31" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="P31" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q31" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="R31" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="S31" s="5"/>
-    </row>
-    <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S31" s="8"/>
+    </row>
+    <row r="32" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>5476</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="8">
         <v>19</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="E32" s="2">
-        <v>55</v>
-      </c>
-      <c r="F32" s="2" t="s">
+      <c r="E32" s="14">
+        <v>55</v>
+      </c>
+      <c r="F32" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="14">
         <v>6</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="M32" s="2">
+      <c r="I32" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="M32" s="14">
         <v>11</v>
       </c>
-      <c r="N32" s="2">
+      <c r="N32" s="14">
         <v>12</v>
       </c>
-      <c r="O32" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P32" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q32" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="S32" s="5"/>
-    </row>
-    <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O32" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="P32" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q32" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="S32" s="8"/>
+    </row>
+    <row r="33" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <v>5476</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="8">
         <v>19</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="G33" s="2">
-        <v>32</v>
-      </c>
-      <c r="H33" s="2" t="s">
+      <c r="G33" s="14">
+        <v>32</v>
+      </c>
+      <c r="H33" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="M33" s="2">
+      <c r="I33" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="M33" s="14">
         <v>10</v>
       </c>
-      <c r="N33" s="2">
+      <c r="N33" s="14">
         <v>3</v>
       </c>
-      <c r="O33" s="2" t="s">
+      <c r="O33" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="P33" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q33" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="S33" s="5"/>
-    </row>
-    <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P33" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q33" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="S33" s="8"/>
+    </row>
+    <row r="34" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <v>5476</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="8">
         <v>19</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="G34" s="2">
-        <v>55</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="S34" s="5"/>
-    </row>
-    <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G34" s="14">
+        <v>55</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="S34" s="8"/>
+    </row>
+    <row r="35" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <v>5476</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="8">
         <v>19</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="14">
         <v>12</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="S35" s="5"/>
-    </row>
-    <row r="36" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I35" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="S35" s="8"/>
+    </row>
+    <row r="36" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <v>5476</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="8">
         <v>19</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="14">
         <v>14</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="S36" s="5"/>
+      <c r="H36" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="S36" s="8"/>
     </row>
     <row r="37" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="12">

</xml_diff>